<commit_message>
Added sorting and subtotals as well as progress bar
</commit_message>
<xml_diff>
--- a/TestFiles/MLSDataSmallTesting.xlsx
+++ b/TestFiles/MLSDataSmallTesting.xlsx
@@ -8,21 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\HatcoFilesClosedProcessor\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91283A45-6BB9-46ED-9732-43CD656D2E17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{02FBC25A-1414-4DDD-AD91-190E3B15B3C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="276" yWindow="648" windowWidth="15360" windowHeight="9024" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HatcoSampleMLSData" sheetId="1" r:id="rId1"/>
     <sheet name="AgentCombined" sheetId="2" r:id="rId2"/>
     <sheet name="BrokerCombined" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="516">
   <si>
     <t>Selling Agent</t>
   </si>
@@ -1570,18 +1579,6 @@
   </si>
   <si>
     <t>Other Agent Office</t>
-  </si>
-  <si>
-    <t>Sample Name</t>
-  </si>
-  <si>
-    <t>Office</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>Add</t>
   </si>
 </sst>
 </file>
@@ -2069,20 +2066,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7231,111 +7222,69 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EEEE7D5-BFEA-4B26-8E17-7E97EC918F7F}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>499</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5" t="s">
+      <c r="O1" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="P1" s="3" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>517</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>518</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="4">
-        <v>43466</v>
-      </c>
-      <c r="G2" s="7">
-        <v>100000</v>
-      </c>
-      <c r="H2" s="3">
-        <v>20190001</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>500</v>
-      </c>
-      <c r="J2" s="3">
-        <v>1</v>
-      </c>
-      <c r="K2" s="3">
-        <v>1</v>
-      </c>
-      <c r="L2" s="3">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>1</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0</v>
-      </c>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7344,100 +7293,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528DEA68-7474-4A34-BD2D-218968A380EB}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="5" t="s">
         <v>499</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="5" t="s">
         <v>509</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="5" t="s">
         <v>512</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="5" t="s">
         <v>513</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>516</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>517</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>518</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>519</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="9">
-        <v>43466</v>
-      </c>
-      <c r="G2" s="12">
-        <v>100000</v>
-      </c>
-      <c r="H2" s="8">
-        <v>20190001</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>500</v>
-      </c>
-      <c r="J2" s="8">
-        <v>1</v>
-      </c>
-      <c r="K2" s="8">
-        <v>1</v>
-      </c>
-      <c r="L2" s="8">
-        <v>0</v>
-      </c>
-      <c r="M2" s="8">
-        <v>1</v>
-      </c>
-      <c r="N2" s="8">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added toggle to ignore Non-MLS Agents
</commit_message>
<xml_diff>
--- a/TestFiles/MLSDataSmallTesting.xlsx
+++ b/TestFiles/MLSDataSmallTesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\HatcoFilesClosedProcessor\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02FBC25A-1414-4DDD-AD91-190E3B15B3C4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3279E67D-F68D-4468-9D55-F5B4794FC1E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HatcoSampleMLSData" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="BrokerCombined" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -7224,8 +7223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EEEE7D5-BFEA-4B26-8E17-7E97EC918F7F}">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7295,8 +7294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528DEA68-7474-4A34-BD2D-218968A380EB}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>